<commit_message>
[feature] Read Excel && Write File Init
</commit_message>
<xml_diff>
--- a/My project/Excel/Test1.xlsx
+++ b/My project/Excel/Test1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\UnityProject\Auto_Excel_Reader\My project\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47023523-65A1-4B15-9E7D-E65605043B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECF7216-58D9-433F-90C7-58A60A2109D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13635" yWindow="2820" windowWidth="12135" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,42 +25,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Age </t>
-  </si>
-  <si>
-    <t>weight</t>
+    <t>int</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>hight</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>bool</t>
   </si>
   <si>
     <t>location</t>
   </si>
   <si>
-    <t>rotation</t>
-  </si>
-  <si>
-    <t>Height</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>float</t>
-  </si>
-  <si>
     <t>vector3</t>
-  </si>
-  <si>
-    <t>TestValue</t>
   </si>
 </sst>
 </file>
@@ -161,7 +158,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -196,7 +193,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -378,85 +375,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I9"/>
+  <dimension ref="A2:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>100001</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>100002</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>100003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>100003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>100004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>100004</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
         <v>100005</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[feature] write data class
</commit_message>
<xml_diff>
--- a/My project/Excel/Test1.xlsx
+++ b/My project/Excel/Test1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\UnityProject\Auto_Excel_Reader\My project\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECF7216-58D9-433F-90C7-58A60A2109D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0B69BC-E65B-4CA8-8798-68A737AA9D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13635" yWindow="2820" windowWidth="12135" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>ID</t>
   </si>
@@ -58,6 +58,15 @@
   </si>
   <si>
     <t>vector3</t>
+  </si>
+  <si>
+    <t>唯一标识</t>
+  </si>
+  <si>
+    <t>名字</t>
+  </si>
+  <si>
+    <t>how old</t>
   </si>
 </sst>
 </file>
@@ -375,14 +384,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
[feature] edit Data Class Name
</commit_message>
<xml_diff>
--- a/My project/Excel/Test1.xlsx
+++ b/My project/Excel/Test1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\UnityProject\Auto_Excel_Reader\My project\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0B69BC-E65B-4CA8-8798-68A737AA9D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C8BC02-68C2-4713-B51C-53AD9DA5F206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13635" yWindow="2820" windowWidth="12135" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>ID</t>
   </si>
@@ -57,9 +57,6 @@
     <t>location</t>
   </si>
   <si>
-    <t>vector3</t>
-  </si>
-  <si>
     <t>唯一标识</t>
   </si>
   <si>
@@ -67,6 +64,15 @@
   </si>
   <si>
     <t>how old</t>
+  </si>
+  <si>
+    <t>Vector3</t>
+  </si>
+  <si>
+    <t>TestValue</t>
+  </si>
+  <si>
+    <t>Vector3[]</t>
   </si>
 </sst>
 </file>
@@ -384,26 +390,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -422,8 +428,11 @@
       <c r="F2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -440,30 +449,33 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>100001</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>100002</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>100003</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>100004</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>100005</v>
       </c>

</xml_diff>